<commit_message>
16/16 Rest and SOAP exercises passed
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/AustralianPostCode/GetAustralianLocationByPostCode/AustralianLocationByPostCode.xlsx
+++ b/src/main/resources/excelsheets/AustralianPostCode/GetAustralianLocationByPostCode/AustralianLocationByPostCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Main</t>
   </si>
@@ -40,6 +40,24 @@
   </si>
   <si>
     <t>/NewDataSet/Table[1]/Location</t>
+  </si>
+  <si>
+    <t>/NewDataSet/Table[2]/Location</t>
+  </si>
+  <si>
+    <t>/NewDataSet/Table[2]/PostCode</t>
+  </si>
+  <si>
+    <t>/NewDataSet/Table[3]/Location</t>
+  </si>
+  <si>
+    <t>/NewDataSet/Table[3]/PostCode</t>
+  </si>
+  <si>
+    <t>/NewDataSet/Table[4]/Location</t>
+  </si>
+  <si>
+    <t>/NewDataSet/Table[4]/PostCode</t>
   </si>
 </sst>
 </file>
@@ -357,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +414,54 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>